<commit_message>
ea team has respective opp and tm
</commit_message>
<xml_diff>
--- a/nfl_Nversion/nfl_game_stats_2024-09-06.xlsx
+++ b/nfl_Nversion/nfl_game_stats_2024-09-06.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>team</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>week</t>
+  </si>
+  <si>
+    <t>opponent</t>
   </si>
   <si>
     <t>Eagles</t>
@@ -577,13 +580,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT3"/>
+  <dimension ref="A1:AU3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:46">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,10 +725,13 @@
       <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:47">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -806,52 +812,52 @@
         <v>1633</v>
       </c>
       <c r="AB2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AD2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AE2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AF2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AH2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AI2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AJ2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AK2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AM2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AN2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AO2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AP2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AQ2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AR2">
         <v>34</v>
@@ -862,10 +868,13 @@
       <c r="AT2">
         <v>1</v>
       </c>
+      <c r="AU2" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:47">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>38</v>
@@ -946,61 +955,64 @@
         <v>1967</v>
       </c>
       <c r="AB3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AD3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AE3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AF3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AH3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AI3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AJ3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AK3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AL3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AM3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AN3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AO3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AP3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AQ3" t="s">
         <v>63</v>
       </c>
       <c r="AR3">
+        <v>29</v>
+      </c>
+      <c r="AS3">
         <v>34</v>
       </c>
-      <c r="AS3">
-        <v>29</v>
-      </c>
       <c r="AT3">
         <v>1</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>